<commit_message>
Image Thumbnail Creation / Multiple Image Upload / Dynamic Item Addition
</commit_message>
<xml_diff>
--- a/docs/info.xlsx
+++ b/docs/info.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="555" windowWidth="14805" windowHeight="8010" tabRatio="419"/>
+    <workbookView xWindow="240" yWindow="1005" windowWidth="14805" windowHeight="8010" tabRatio="419"/>
   </bookViews>
   <sheets>
     <sheet name="Website timeline" sheetId="1" r:id="rId1"/>
-    <sheet name="Tasks" sheetId="4" r:id="rId2"/>
-    <sheet name="Details to enter for diamonds" sheetId="3" r:id="rId3"/>
+    <sheet name="Daily Progress" sheetId="5" r:id="rId2"/>
+    <sheet name="Tasks" sheetId="4" r:id="rId3"/>
+    <sheet name="Details to enter for diamonds" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="60">
   <si>
     <t>Work</t>
   </si>
@@ -181,6 +182,21 @@
   </si>
   <si>
     <t>Done</t>
+  </si>
+  <si>
+    <t>Login page</t>
+  </si>
+  <si>
+    <t>Registration</t>
+  </si>
+  <si>
+    <t>Front lane dynamic</t>
+  </si>
+  <si>
+    <t>Dynamic Jewelery lane minimum working</t>
+  </si>
+  <si>
+    <t>Multiple Image Upload + Image Thumbnail Creation</t>
   </si>
 </sst>
 </file>
@@ -278,7 +294,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -287,6 +303,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -591,10 +608,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -725,7 +742,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
-        <v>14</v>
+        <v>58</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>13</v>
@@ -745,35 +762,25 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="3">
-        <v>2</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="D11" s="3">
         <v>2</v>
       </c>
-      <c r="E11" s="4">
-        <v>42607</v>
-      </c>
-      <c r="F11" s="7">
-        <v>42608</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>27</v>
-      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D12" s="3">
         <v>2</v>
@@ -790,45 +797,51 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="D13" s="3">
         <v>2</v>
       </c>
+      <c r="E13" s="4">
+        <v>42607</v>
+      </c>
+      <c r="F13" s="7">
+        <v>42608</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D14" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D15" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" s="3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="3" t="s">
-        <v>20</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>13</v>
@@ -837,37 +850,51 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="D18" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="3" t="s">
-        <v>25</v>
       </c>
       <c r="D19" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D20" s="3">
+      <c r="D21" s="3">
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="3" t="s">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="3" t="s">
+      <c r="H22" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="3" t="s">
         <v>53</v>
       </c>
     </row>
@@ -878,6 +905,44 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:A5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8">
+        <v>42607</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
@@ -953,7 +1018,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:B11"/>
   <sheetViews>

</xml_diff>

<commit_message>
info updated: multi lingual option
</commit_message>
<xml_diff>
--- a/docs/info.xlsx
+++ b/docs/info.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="62">
   <si>
     <t>Work</t>
   </si>
@@ -200,6 +200,9 @@
   </si>
   <si>
     <t>Session management</t>
+  </si>
+  <si>
+    <t>Multi-lingual option</t>
   </si>
 </sst>
 </file>
@@ -611,10 +614,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -970,6 +973,14 @@
       </c>
       <c r="B24" s="3" t="s">
         <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" s="3">
+        <v>23</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
action point on karan to install centos
</commit_message>
<xml_diff>
--- a/docs/info.xlsx
+++ b/docs/info.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="66">
   <si>
     <t>Work</t>
   </si>
@@ -212,6 +212,9 @@
   </si>
   <si>
     <t>Testsite authentication flag &amp; box</t>
+  </si>
+  <si>
+    <t>Install CentOS 6 + LAMP</t>
   </si>
 </sst>
 </file>
@@ -623,10 +626,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1017,6 +1020,17 @@
       </c>
       <c r="B28" s="3" t="s">
         <v>64</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" s="3">
+        <v>27</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Products upload excel sheet format
</commit_message>
<xml_diff>
--- a/docs/info.xlsx
+++ b/docs/info.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="1008" windowWidth="14808" windowHeight="8016" tabRatio="419"/>
+    <workbookView xWindow="240" yWindow="1008" windowWidth="14808" windowHeight="8016" tabRatio="545"/>
   </bookViews>
   <sheets>
     <sheet name="Website timeline" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="67">
   <si>
     <t>Work</t>
   </si>
@@ -215,6 +215,9 @@
   </si>
   <si>
     <t>Link to download centos6:</t>
+  </si>
+  <si>
+    <t>New mysql tables required for excel upload (check Products upload excel file)</t>
   </si>
 </sst>
 </file>
@@ -626,10 +629,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J33"/>
+  <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1101,6 +1104,17 @@
         <v>25</v>
       </c>
     </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" s="3">
+        <v>32</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -1140,7 +1154,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:D6"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>